<commit_message>
Standardized the file format and completed the experimental document.
</commit_message>
<xml_diff>
--- a/3.b.TF-IDF/splitTF-IDFCluster/cluster_0.xlsx
+++ b/3.b.TF-IDF/splitTF-IDFCluster/cluster_0.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:F42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -437,436 +437,681 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
+          <t>id</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>category</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>severity</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>recurrent</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
           <t>result</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="F1" s="1" t="inlineStr">
         <is>
           <t>processed_result</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>category</t>
-        </is>
-      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" t="n">
+        <v>10010000009058</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>安全</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>5</v>
+      </c>
+      <c r="D2" t="n">
+        <v>5</v>
+      </c>
+      <c r="E2" t="inlineStr">
         <is>
           <t>在清空聊天记录后，用户试图查看聊天记录时发现聊天记录仍然存在，与预期的“已清空”不符。</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="F2" t="inlineStr">
         <is>
           <t>清空 聊天记录 试图 查看 聊天记录 发现 聊天记录 仍然 预期 清空 不符</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>安全</t>
-        </is>
-      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" t="n">
+        <v>10010000008776</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>功能不完整</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" t="n">
+        <v>5</v>
+      </c>
+      <c r="E3" t="inlineStr">
         <is>
           <t>在群聊或私聊的聊天界面中，当用户删除了聊天记录后，再次进入该界面时，尽管聊天记录已被清除，但历史消息部分仍然显示之前的聊天记录。这意味着即使用户已经删除了消息，系统并没有正确地更新消息记录，导致功能不完整。</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="F3" t="inlineStr">
         <is>
           <t>群聊 私聊 聊天 界面 删除 聊天记录 再次 进入 界面 聊天记录 清除 历史 消息 部分 仍然 之前 聊天记录 意味着 删除 消息 系统 没有 正确 更新 消息 记录 完整</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>10010000007947</v>
+      </c>
+      <c r="B4" t="inlineStr">
         <is>
           <t>功能不完整</t>
         </is>
       </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="C4" t="n">
+        <v>3</v>
+      </c>
+      <c r="D4" t="n">
+        <v>5</v>
+      </c>
+      <c r="E4" t="inlineStr">
         <is>
           <t>在查询聊天记录时，用户输入关键字后，系统没有返回任何提示信息。尽管本地记录中存在相应的聊天内容，但查询结果仍然为空，导致用户无法找到他们想要查找的聊天记录。</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="F4" t="inlineStr">
         <is>
           <t>查询 聊天记录 输入 关键字 系统 没有 返回 提示信息 记录 相应 聊天 内容 查询 仍然 为空 无法 找到 想要 查找 聊天记录</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>10010000009495</v>
+      </c>
+      <c r="B5" t="inlineStr">
         <is>
           <t>功能不完整</t>
         </is>
       </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>1</v>
+      </c>
+      <c r="E5" t="inlineStr">
         <is>
           <t>该软件在执行“清空聊天记录”的操作后，未能完全删除历史消息。尽管用户尝试通过界面选项来清除聊天记录，但在聊天历史中仍然可以找到被删除的消息，这表明软件的聊天记录清理功能存在缺陷。</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="F5" t="inlineStr">
         <is>
           <t>执行 清空 聊天记录 未能 完全 删除 历史 消息 界面 选项 清除 聊天记录 聊天 历史 仍然 找到 删除 消息 表明 软件 聊天记录 清理 缺陷</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>10010000009279</v>
+      </c>
+      <c r="B6" t="inlineStr">
         <is>
           <t>功能不完整</t>
         </is>
       </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="C6" t="n">
+        <v>2</v>
+      </c>
+      <c r="D6" t="n">
+        <v>5</v>
+      </c>
+      <c r="E6" t="inlineStr">
         <is>
           <t>在与好友的聊天记录界面，点击下载语音文件无法下载，而是弹出试听</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr">
+      <c r="F6" t="inlineStr">
         <is>
           <t>好友 聊天记录 界面 点击 下载 语音 文件 无法 下载 弹 出 试听</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>10010000008342</v>
+      </c>
+      <c r="B7" t="inlineStr">
         <is>
           <t>功能不完整</t>
         </is>
       </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="C7" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" t="n">
+        <v>5</v>
+      </c>
+      <c r="E7" t="inlineStr">
         <is>
           <t>该软件在查看历史消息时存在一个明显的bug。当用户按时间查找并点击没有聊天记录的时间点时，系统并未给出预期的提示信息，表明没有聊天记录。此外，选择时间的交互方式并不友好，可能导致用户误操作或难以理解如何进行下一步操作。</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="F7" t="inlineStr">
         <is>
           <t>查看 历史 消息 明显 时间 查找 点击 没有 聊天记录 时间 点时 系统 并未 给出 预期 提示信息 表明 没有 聊天记录 选择 时间 交互方式 友好 误操作 难以 理解 进行 一步</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>10010000009616</v>
+      </c>
+      <c r="B8" t="inlineStr">
         <is>
           <t>功能不完整</t>
         </is>
       </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="C8" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" t="n">
+        <v>5</v>
+      </c>
+      <c r="E8" t="inlineStr">
         <is>
           <t>该问题描述了一个软件的bug，即在删除群内聊天记录后，用户仍然可以在历史记录中找到这些已被删除的聊天记录。</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="F8" t="inlineStr">
         <is>
           <t>软件 删除 群内 聊天记录 仍然 历史记录 找到 删除 聊天记录</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
+    </row>
+    <row r="9">
+      <c r="A9" t="n">
+        <v>10010000008370</v>
+      </c>
+      <c r="B9" t="inlineStr">
         <is>
           <t>功能不完整</t>
         </is>
       </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="C9" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" t="n">
+        <v>5</v>
+      </c>
+      <c r="E9" t="inlineStr">
         <is>
           <t>该软件在客户端被卸载并重新安装后，聊天记录未能正确更新，仍显示为在软件卸载前与某个好友的聊天记录。这导致用户无法查看和交互最新的聊天信息。</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="F9" t="inlineStr">
         <is>
           <t>客户端 卸载 重新安装 聊天记录 未能 正确 更新 软件 卸载 前 好友 聊天记录 无法 查看 交互 最新 聊天 信息</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
+    </row>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>10010000008374</v>
+      </c>
+      <c r="B10" t="inlineStr">
         <is>
           <t>功能不完整</t>
         </is>
       </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="C10" t="n">
+        <v>4</v>
+      </c>
+      <c r="D10" t="n">
+        <v>5</v>
+      </c>
+      <c r="E10" t="inlineStr">
         <is>
           <t>在群聊中尝试清空聊天记录时，尽管已执行相关操作，但群成员仍能看到部分历史消息。</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="F10" t="inlineStr">
         <is>
           <t>群聊 清空 聊天记录 执行 相关 但群 成员 仍能 看到 部分 历史 消息</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>10010000008495</v>
+      </c>
+      <c r="B11" t="inlineStr">
         <is>
           <t>功能不完整</t>
         </is>
       </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
+      <c r="C11" t="n">
+        <v>5</v>
+      </c>
+      <c r="D11" t="n">
+        <v>5</v>
+      </c>
+      <c r="E11" t="inlineStr">
         <is>
           <t>该软件中存在一个bug，即在群聊中用户尝试清空聊天记录后，当他们再次点击聊天记录时，之前的聊天记录仍然会重新出现，没有达到预期的“清空”效果。</t>
         </is>
       </c>
-      <c r="B11" t="inlineStr">
+      <c r="F11" t="inlineStr">
         <is>
           <t>群聊 清空 聊天记录 再次 点击 聊天记录 之前 聊天记录 仍然 重新 出现 没有 达到 预期 清空 效果</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>10010000008520</v>
+      </c>
+      <c r="B12" t="inlineStr">
         <is>
           <t>功能不完整</t>
         </is>
       </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
+      <c r="C12" t="n">
+        <v>4</v>
+      </c>
+      <c r="D12" t="n">
+        <v>5</v>
+      </c>
+      <c r="E12" t="inlineStr">
         <is>
           <t>该bug描述了一个软件功能异常的问题。在用户尝试清空聊天记录时，虽然聊天记录已被成功删除，但用户仍然可以通过查看消息列表来访问并查看以前的聊天记录。这违反了用户期望的清空操作的结果，可能导致隐私泄露或误导性信息展示。</t>
         </is>
       </c>
-      <c r="B12" t="inlineStr">
+      <c r="F12" t="inlineStr">
         <is>
           <t>软件 异常 清空 聊天记录 聊天记录 成功 删除 仍然 查看 消息 列表 访问 查看 以前 聊天记录 违反 期望 清空 隐私 泄露 误导性 信息 展示</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>10010000009701</v>
+      </c>
+      <c r="B13" t="inlineStr">
         <is>
           <t>功能不完整</t>
         </is>
       </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
+      <c r="C13" t="n">
+        <v>3</v>
+      </c>
+      <c r="D13" t="n">
+        <v>3</v>
+      </c>
+      <c r="E13" t="inlineStr">
         <is>
           <t>群聊里面的聊天记录保存的比较少，而且页面太大，布局不好</t>
         </is>
       </c>
-      <c r="B13" t="inlineStr">
+      <c r="F13" t="inlineStr">
         <is>
           <t>群聊 里面 聊天记录 保存 比较 少 页面 太 布局 不好</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>10010000009625</v>
+      </c>
+      <c r="B14" t="inlineStr">
         <is>
           <t>功能不完整</t>
         </is>
       </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
+      <c r="C14" t="n">
+        <v>3</v>
+      </c>
+      <c r="D14" t="n">
+        <v>5</v>
+      </c>
+      <c r="E14" t="inlineStr">
         <is>
           <t>该软件存在一个明显的bug。用户在群组设置中点击清空聊天记录后，本应清空的聊天记录在聊天记录里仍然可以查看，这违反了用户的预期行为。按照正常的功能设计，用户点击清空聊天记录后，该部分记录应该被删除，无法再次查看。然而，在这个软件中，尽管用户已经执行了清空操作，但聊天记录页面依然保留并显示了聊天记录，这显然是一个功能故障。</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
+      <c r="F14" t="inlineStr">
         <is>
           <t>明显 群组 设置 点击 清空 聊天记录 本应 清空 聊天记录 聊天记录 里 仍然 查看 违反 预期 行为 正常 功能设计 点击 清空 聊天记录 部分 记录 应该 删除 无法 再次 查看 软件 执行 清空 聊天记录 页面 依然 保留 聊天记录 显然 故障</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>10010000009694</v>
+      </c>
+      <c r="B15" t="inlineStr">
         <is>
           <t>功能不完整</t>
         </is>
       </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
+      <c r="C15" t="n">
+        <v>4</v>
+      </c>
+      <c r="D15" t="n">
+        <v>5</v>
+      </c>
+      <c r="E15" t="inlineStr">
         <is>
           <t>如之前的聊天记录是空的并不会提示之前的聊天记录无。而是显示今天的聊天记录。但查找今天以后的聊天记录就会显示无。
 如下图所示  我查找的是12月1日的聊天记录 却显示的12月3日的</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>之前 聊天记录 空 不会 提示 之前 聊天记录 今天 聊天记录 查找 今天 以后 聊天记录 
  图 所示     查找 12 月 日 聊天记录   12 月 日</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
+    </row>
+    <row r="16">
+      <c r="A16" t="n">
+        <v>10010000009445</v>
+      </c>
+      <c r="B16" t="inlineStr">
         <is>
           <t>功能不完整</t>
         </is>
       </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
+      <c r="C16" t="n">
+        <v>3</v>
+      </c>
+      <c r="D16" t="n">
+        <v>5</v>
+      </c>
+      <c r="E16" t="inlineStr">
         <is>
           <t>1.测试功能：聊天页面删除功能
 2.实际结果：无法删除任何聊天记录
 3.预期结果：可随意删除群组聊天与好友聊天</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>. 聊天 页面 删除 
  . 无法 删除 聊天记录 
  . 预期 随意 删除 群组 聊天 好友 聊天</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
+    </row>
+    <row r="17">
+      <c r="A17" t="n">
+        <v>10010000009138</v>
+      </c>
+      <c r="B17" t="inlineStr">
         <is>
           <t>功能不完整</t>
         </is>
       </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="inlineStr">
+      <c r="C17" t="n">
+        <v>3</v>
+      </c>
+      <c r="D17" t="n">
+        <v>5</v>
+      </c>
+      <c r="E17" t="inlineStr">
         <is>
           <t>在聊天记录页面中，当用户尝试删除特定的聊天记录后，再次查询时发现被删除的记录仍然存在于列表中。这显示了一个明显的bug，即删除操作并未正确地更新数据库或内存中的记录状态。</t>
         </is>
       </c>
-      <c r="B17" t="inlineStr">
+      <c r="F17" t="inlineStr">
         <is>
           <t>聊天记录 页面 删除 特定 聊天记录 再次 查询 发现 删除 记录 仍然 列表 明显 删除 并未 正确 更新 数据库 内存 记录 状态</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
+    </row>
+    <row r="18">
+      <c r="A18" t="n">
+        <v>10010000009568</v>
+      </c>
+      <c r="B18" t="inlineStr">
         <is>
           <t>功能不完整</t>
         </is>
       </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
+      <c r="C18" t="n">
+        <v>4</v>
+      </c>
+      <c r="D18" t="n">
+        <v>5</v>
+      </c>
+      <c r="E18" t="inlineStr">
         <is>
           <t>此软件在处理日期输入时存在逻辑错误。当用户尝试查询特定日期（2016年12月3日）的聊天记录时，软件正确地返回了该日期的消息，这与预期输出一致。然而，当用户尝试查询非特定日期（例如2015年12月2日或之前的所有日期）的聊天记录时，软件返回了大量非当天的聊天记录，这与预期输出不符。此外，与前一个bug相似，无论用户何时查询聊天记录，结果都会包含大量非当天的记录，这显然是不符合需求的。</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>软件 处理 日期 输入 逻辑 错误 查询 特定 日期 2016 年 12 月 日 聊天记录 软件 正确 返回 日期 消息 预期 输出 一致 查询 非 特定 日期 2015 年 12 月 日 之前 日期 聊天记录 软件 返回 大量 非 当天 聊天记录 预期 输出 不符 前 相似 查询 聊天记录 包含 大量 非 当天 记录 显然 符合 需求</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
+    </row>
+    <row r="19">
+      <c r="A19" t="n">
+        <v>10010000009767</v>
+      </c>
+      <c r="B19" t="inlineStr">
         <is>
           <t>功能不完整</t>
         </is>
       </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="inlineStr">
+      <c r="C19" t="n">
+        <v>1</v>
+      </c>
+      <c r="D19" t="n">
+        <v>5</v>
+      </c>
+      <c r="E19" t="inlineStr">
         <is>
           <t>该软件的聊天记录删除功能存在bug，用户在删除群聊天记录后，这些记录依然可见。</t>
         </is>
       </c>
-      <c r="B19" t="inlineStr">
+      <c r="F19" t="inlineStr">
         <is>
           <t>聊天记录 删除 删除 群 聊天记录 记录 依然</t>
         </is>
       </c>
-      <c r="C19" t="inlineStr">
+    </row>
+    <row r="20">
+      <c r="A20" t="n">
+        <v>10010000009861</v>
+      </c>
+      <c r="B20" t="inlineStr">
         <is>
           <t>功能不完整</t>
         </is>
       </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="inlineStr">
+      <c r="C20" t="n">
+        <v>1</v>
+      </c>
+      <c r="D20" t="n">
+        <v>5</v>
+      </c>
+      <c r="E20" t="inlineStr">
         <is>
           <t>在聊天记录查找功能中存在一个bug，用户无法根据指定内容进行搜索。</t>
         </is>
       </c>
-      <c r="B20" t="inlineStr">
+      <c r="F20" t="inlineStr">
         <is>
           <t>聊天记录 查找 无法 指定 内容 进行 搜索</t>
         </is>
       </c>
-      <c r="C20" t="inlineStr">
+    </row>
+    <row r="21">
+      <c r="A21" t="n">
+        <v>10010000009898</v>
+      </c>
+      <c r="B21" t="inlineStr">
         <is>
           <t>功能不完整</t>
         </is>
       </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="inlineStr">
+      <c r="C21" t="n">
+        <v>1</v>
+      </c>
+      <c r="D21" t="n">
+        <v>5</v>
+      </c>
+      <c r="E21" t="inlineStr">
         <is>
           <t>该软件的群聊历史记录功能存在一个bug，用户无法通过日期查找聊天记录。</t>
         </is>
       </c>
-      <c r="B21" t="inlineStr">
+      <c r="F21" t="inlineStr">
         <is>
           <t>群聊 历史记录 无法 日期 查找 聊天记录</t>
         </is>
       </c>
-      <c r="C21" t="inlineStr">
+    </row>
+    <row r="22">
+      <c r="A22" t="n">
+        <v>10010000009529</v>
+      </c>
+      <c r="B22" t="inlineStr">
         <is>
           <t>功能不完整</t>
         </is>
       </c>
-    </row>
-    <row r="22">
-      <c r="A22" t="inlineStr">
+      <c r="C22" t="n">
+        <v>4</v>
+      </c>
+      <c r="D22" t="n">
+        <v>4</v>
+      </c>
+      <c r="E22" t="inlineStr">
         <is>
           <t>在群设置中，清空聊天记录后，聊天记录中仍存在部分内容未被删除。</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="F22" t="inlineStr">
         <is>
           <t>群 设置 清空 聊天记录 聊天记录 部分 内容 未 删除</t>
         </is>
       </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>功能不完整</t>
-        </is>
-      </c>
     </row>
     <row r="23">
-      <c r="A23" t="inlineStr">
+      <c r="A23" t="n">
+        <v>10010000009794</v>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>性能</t>
+        </is>
+      </c>
+      <c r="C23" t="n">
+        <v>3</v>
+      </c>
+      <c r="D23" t="n">
+        <v>5</v>
+      </c>
+      <c r="E23" t="inlineStr">
         <is>
           <t>在软件的管理员审批功能中，存在一个明显的界面和逻辑错误。当用户尝试发起聊天或查看聊天记录时，系统似乎无法正常显示这些信息。此外，审批状态的百分比显示为87%，这可能意味着该功能的某些部分已经成功执行，但整体上可能存在问题。</t>
         </is>
       </c>
-      <c r="B23" t="inlineStr">
+      <c r="F23" t="inlineStr">
         <is>
           <t>软件 管理员 审批 明显 界面 逻辑 错误 发起 聊天 查看 聊天记录 系统 无法 正常 信息 审批 状态 百分比 87% 意味着 部分 成功 执行 整体</t>
         </is>
       </c>
-      <c r="C23" t="inlineStr">
+    </row>
+    <row r="24">
+      <c r="A24" t="n">
+        <v>10010000009110</v>
+      </c>
+      <c r="B24" t="inlineStr">
         <is>
           <t>性能</t>
         </is>
       </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
+      <c r="C24" t="n">
+        <v>1</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" t="inlineStr">
         <is>
           <t>这个bug是关于一个群聊的设置功能，当用户点击群设置里的“查看聊天记录”时，系统应该允许用户按时间顺序查看过去的聊天记录。但在当前的界面设计中，该功能似乎无法正常工作或展示出正确的时间排序，导致用户无法按照预期的方式查看聊天记录。</t>
         </is>
       </c>
-      <c r="B24" t="inlineStr">
+      <c r="F24" t="inlineStr">
         <is>
           <t>群聊 设置 点击 群 设置 里 查看 聊天记录 系统 应该 允许 时间 顺序 查看 过去 聊天记录 当前 界面设计 无法 正常 工作 展示 出 正确 时间 排序 无法 预期 方式 查看 聊天记录</t>
         </is>
       </c>
-      <c r="C24" t="inlineStr">
+    </row>
+    <row r="25">
+      <c r="A25" t="n">
+        <v>10010000009177</v>
+      </c>
+      <c r="B25" t="inlineStr">
         <is>
           <t>性能</t>
         </is>
       </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
+      <c r="C25" t="n">
+        <v>3</v>
+      </c>
+      <c r="D25" t="n">
+        <v>1</v>
+      </c>
+      <c r="E25" t="inlineStr">
         <is>
           <t>该软件的“清空聊天记录”功能似乎没有按预期工作。尽管在点击后聊天记录显示为已清空，但用户仍可以通过查看聊天记录来访问这些信息。这可能表明软件并未真正删除聊天记录，或者存在某种数据残留或错误。</t>
         </is>
       </c>
-      <c r="B25" t="inlineStr">
+      <c r="F25" t="inlineStr">
         <is>
           <t>清空 聊天记录 没有 预期 工作 点击 聊天记录 清空 查看 聊天记录 访问 信息 表明 软件 并未 真正 删除 聊天记录 某种 数据 残留 错误</t>
         </is>
       </c>
-      <c r="C25" t="inlineStr">
+    </row>
+    <row r="26">
+      <c r="A26" t="n">
+        <v>10010000009546</v>
+      </c>
+      <c r="B26" t="inlineStr">
         <is>
           <t>性能</t>
         </is>
       </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
+      <c r="C26" t="n">
+        <v>4</v>
+      </c>
+      <c r="D26" t="n">
+        <v>5</v>
+      </c>
+      <c r="E26" t="inlineStr">
         <is>
           <t>1.查看聊天记录
 2.步骤重现：群组或好友聊天界面点击右上角-聊天记录
@@ -874,7 +1119,7 @@
 4.预期结果：聊天记录较为完全，保存最近的聊天结果，查看的结果应比聊天界面显示的结果多</t>
         </is>
       </c>
-      <c r="B26" t="inlineStr">
+      <c r="F26" t="inlineStr">
         <is>
           <t>. 查看 聊天记录 
  . 重现 群组 好友 聊天 界面 点击 右上角 - 聊天记录 
@@ -882,281 +1127,420 @@
  . 预期 聊天记录 较为 完全 保存 最近 聊天 查看 应比 聊天 界面显示</t>
         </is>
       </c>
-      <c r="C26" t="inlineStr">
+    </row>
+    <row r="27">
+      <c r="A27" t="n">
+        <v>10010000008988</v>
+      </c>
+      <c r="B27" t="inlineStr">
         <is>
           <t>性能</t>
         </is>
       </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
+      <c r="C27" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" t="n">
+        <v>2</v>
+      </c>
+      <c r="E27" t="inlineStr">
         <is>
           <t>在历史聊天记录界面中，用户尝试进行关键字查询搜索时，发现加载时间过长，无法在短时间内获取查询结果。这可能导致用户体验下降，影响用户的使用效率和满意度。</t>
         </is>
       </c>
-      <c r="B27" t="inlineStr">
+      <c r="F27" t="inlineStr">
         <is>
           <t>历史 聊天记录 界面 进行 关键字 查询 搜索 发现 加载 时间 过长 无法 短时间 获取 查询 下降 效率 满意度</t>
         </is>
       </c>
-      <c r="C27" t="inlineStr">
+    </row>
+    <row r="28">
+      <c r="A28" t="n">
+        <v>10010000009127</v>
+      </c>
+      <c r="B28" t="inlineStr">
         <is>
           <t>性能</t>
         </is>
       </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
+      <c r="C28" t="n">
+        <v>2</v>
+      </c>
+      <c r="D28" t="n">
+        <v>1</v>
+      </c>
+      <c r="E28" t="inlineStr">
         <is>
           <t>在聊天记录界面，信息显示不全，导致部分聊天内容丢失。</t>
         </is>
       </c>
-      <c r="B28" t="inlineStr">
+      <c r="F28" t="inlineStr">
         <is>
           <t>聊天记录 界面 信息 不全 部分 聊天 内容 丢失</t>
         </is>
       </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>性能</t>
-        </is>
-      </c>
     </row>
     <row r="29">
-      <c r="A29" t="inlineStr">
+      <c r="A29" t="n">
+        <v>10010000008328</v>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>页面布局缺陷</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>3</v>
+      </c>
+      <c r="D29" t="n">
+        <v>5</v>
+      </c>
+      <c r="E29" t="inlineStr">
         <is>
           <t>用户进入群“聊天记录”，上面的搜索按钮出现了两个，页面布局有误</t>
         </is>
       </c>
-      <c r="B29" t="inlineStr">
+      <c r="F29" t="inlineStr">
         <is>
           <t>进入 群 聊天记录 上面 搜索 按钮 出现 两个 页面 布局 有误</t>
         </is>
       </c>
-      <c r="C29" t="inlineStr">
+    </row>
+    <row r="30">
+      <c r="A30" t="n">
+        <v>10010000009436</v>
+      </c>
+      <c r="B30" t="inlineStr">
         <is>
           <t>页面布局缺陷</t>
         </is>
       </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
+      <c r="C30" t="n">
+        <v>3</v>
+      </c>
+      <c r="D30" t="n">
+        <v>5</v>
+      </c>
+      <c r="E30" t="inlineStr">
         <is>
           <t>在华为P7手机上，进入群聊中的聊天记录页面时，搜索图标的UI层面显示有误。</t>
         </is>
       </c>
-      <c r="B30" t="inlineStr">
+      <c r="F30" t="inlineStr">
         <is>
           <t>华为 P7 手机 进入 群聊 聊天记录 页面 搜索 图标 UI 层面 有误</t>
         </is>
       </c>
-      <c r="C30" t="inlineStr">
+    </row>
+    <row r="31">
+      <c r="A31" t="n">
+        <v>10010000009306</v>
+      </c>
+      <c r="B31" t="inlineStr">
         <is>
           <t>页面布局缺陷</t>
         </is>
       </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
+      <c r="C31" t="n">
+        <v>5</v>
+      </c>
+      <c r="D31" t="n">
+        <v>5</v>
+      </c>
+      <c r="E31" t="inlineStr">
         <is>
           <t>在群设置中 点击聊天记录 之后再历史消息中点击查看更多消息之后往下翻 就会发现 聊天记录时间抽错乱 如下图所示</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="F31" t="inlineStr">
         <is>
           <t>群 设置   点击 聊天记录   之后 历史 消息 点击 查看 更 消息 之后 往下 翻   发现   聊天记录 时间 抽 错乱   图 所示</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
+    </row>
+    <row r="32">
+      <c r="A32" t="n">
+        <v>10010000009087</v>
+      </c>
+      <c r="B32" t="inlineStr">
         <is>
           <t>页面布局缺陷</t>
         </is>
       </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
+      <c r="C32" t="n">
+        <v>3</v>
+      </c>
+      <c r="D32" t="n">
+        <v>5</v>
+      </c>
+      <c r="E32" t="inlineStr">
         <is>
           <t>该软件界面显示了聊天记录的搜索功能，但存在视觉和功能上的问题。在查看聊天记录时，两个搜索标志重叠在一起，导致用户难以区分并使用它们。这可能是由于设计错误或布局问题导致的冗余显示。</t>
         </is>
       </c>
-      <c r="B32" t="inlineStr">
+      <c r="F32" t="inlineStr">
         <is>
           <t>界面显示 聊天记录 搜索 视觉 查看 聊天记录 两个 搜索 标志 重叠 一起 难以 区分 设计 错误 布局 冗余</t>
         </is>
       </c>
-      <c r="C32" t="inlineStr">
+    </row>
+    <row r="33">
+      <c r="A33" t="n">
+        <v>10010000009671</v>
+      </c>
+      <c r="B33" t="inlineStr">
         <is>
           <t>页面布局缺陷</t>
         </is>
       </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
+      <c r="C33" t="n">
+        <v>3</v>
+      </c>
+      <c r="D33" t="n">
+        <v>1</v>
+      </c>
+      <c r="E33" t="inlineStr">
         <is>
           <t>在聊天记录界面中，图片之间的布局和间距显得混乱，导致用户难以区分和识别不同的消息内容。</t>
         </is>
       </c>
-      <c r="B33" t="inlineStr">
+      <c r="F33" t="inlineStr">
         <is>
           <t>聊天记录 界面 图片 之间 布局 间距 显得 混乱 难以 区分 识别 不同 消息 内容</t>
         </is>
       </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>页面布局缺陷</t>
-        </is>
-      </c>
     </row>
     <row r="34">
-      <c r="A34" t="inlineStr">
+      <c r="A34" t="n">
+        <v>10010000008324</v>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>用户体验</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>3</v>
+      </c>
+      <c r="D34" t="n">
+        <v>5</v>
+      </c>
+      <c r="E34" t="inlineStr">
         <is>
           <t>删除好友后，最近联系人列表中仍然存在被删用户和聊天记录的显示问题。在尝试清除与该用户的联系后，相关数据并未从界面上移除，导致信息显示不一致。</t>
         </is>
       </c>
-      <c r="B34" t="inlineStr">
+      <c r="F34" t="inlineStr">
         <is>
           <t>删除 好友 最近 联系人 列表 仍然 被删 聊天记录 清除 联系 相关 数据 并未 界面 上移 信息 一致</t>
         </is>
       </c>
-      <c r="C34" t="inlineStr">
+    </row>
+    <row r="35">
+      <c r="A35" t="n">
+        <v>10010000009805</v>
+      </c>
+      <c r="B35" t="inlineStr">
         <is>
           <t>用户体验</t>
         </is>
       </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
+      <c r="C35" t="n">
+        <v>3</v>
+      </c>
+      <c r="D35" t="n">
+        <v>3</v>
+      </c>
+      <c r="E35" t="inlineStr">
         <is>
           <t>该软件的聊天记录显示功能存在bug。在用户尝试查看“查看更多消息”时，聊天记录会重复显示，导致信息冗余，这可能会干扰用户对历史消息的理解，影响用户体验。</t>
         </is>
       </c>
-      <c r="B35" t="inlineStr">
+      <c r="F35" t="inlineStr">
         <is>
           <t>聊天记录 查看 查看 更 消息 聊天记录 重复 信息冗余 干扰 历史 消息 理解</t>
         </is>
       </c>
-      <c r="C35" t="inlineStr">
+    </row>
+    <row r="36">
+      <c r="A36" t="n">
+        <v>10010000009237</v>
+      </c>
+      <c r="B36" t="inlineStr">
         <is>
           <t>用户体验</t>
         </is>
       </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
+      <c r="C36" t="n">
+        <v>3</v>
+      </c>
+      <c r="D36" t="n">
+        <v>5</v>
+      </c>
+      <c r="E36" t="inlineStr">
         <is>
           <t>随着聊天记录的增加，群公告会移到上面去，不利于消息的通知</t>
         </is>
       </c>
-      <c r="B36" t="inlineStr">
+      <c r="F36" t="inlineStr">
         <is>
           <t>聊天记录 增加 群 公告 会移 上面 不利于 消息 通知</t>
         </is>
       </c>
-      <c r="C36" t="inlineStr">
+    </row>
+    <row r="37">
+      <c r="A37" t="n">
+        <v>10010000008204</v>
+      </c>
+      <c r="B37" t="inlineStr">
         <is>
           <t>用户体验</t>
         </is>
       </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
+      <c r="C37" t="n">
+        <v>1</v>
+      </c>
+      <c r="D37" t="n">
+        <v>5</v>
+      </c>
+      <c r="E37" t="inlineStr">
         <is>
           <t>在软件测试过程中，发现一个页面元素混乱的问题。当用户尝试通过关键字查找聊天记录时，如果找不到相应的记录，删除搜索框中的关键字后，下方的显示区域并未回到初始的“显示全部聊天记录”状态，而是仍然为空白，这可能给用户带来困扰和不便。</t>
         </is>
       </c>
-      <c r="B37" t="inlineStr">
+      <c r="F37" t="inlineStr">
         <is>
           <t>软件测试 过程 发现 页面 元素 混乱 关键字 查找 聊天记录 找 不到 相应 记录 删除 搜索 框中 关键字 下方 区域 并未 回到 初始 聊天记录 状态 仍然 空白 带来 困扰 不便</t>
         </is>
       </c>
-      <c r="C37" t="inlineStr">
+    </row>
+    <row r="38">
+      <c r="A38" t="n">
+        <v>10010000009382</v>
+      </c>
+      <c r="B38" t="inlineStr">
         <is>
           <t>用户体验</t>
         </is>
       </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
+      <c r="C38" t="n">
+        <v>3</v>
+      </c>
+      <c r="D38" t="n">
+        <v>5</v>
+      </c>
+      <c r="E38" t="inlineStr">
         <is>
           <t>该界面显示的是一个手机聊天应用的历史消息页面。页面顶部有一个返回箭头，旁边是“历史消息”四个字。屏幕中部有两个搜索按钮，一个标有“全部”，另一个标有“你好”。在这两个按钮下方，显示了一条聊天记录的日期和时间：“2016-12-03”。最下方的文字“加载中…”表明当前没有聊天记录可见，可能是正在加载或数据尚未更新。</t>
         </is>
       </c>
-      <c r="B38" t="inlineStr">
+      <c r="F38" t="inlineStr">
         <is>
           <t>界面显示 手机 聊天 应用 历史 消息 页面 页面 顶部 返回 箭头 旁边 历史 消息 四个 字 屏幕 中部 两个 搜索 按钮 标有 标有 你好 两个 按钮 下方 一条 聊天记录 日期 时间 2016 - 12 - 03 下方 文字 加载 … 表明 当前 没有 聊天记录 正在 加载 数据 尚未 更新</t>
         </is>
       </c>
-      <c r="C38" t="inlineStr">
+    </row>
+    <row r="39">
+      <c r="A39" t="n">
+        <v>10010000008994</v>
+      </c>
+      <c r="B39" t="inlineStr">
         <is>
           <t>用户体验</t>
         </is>
       </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
+      <c r="C39" t="n">
+        <v>3</v>
+      </c>
+      <c r="D39" t="n">
+        <v>5</v>
+      </c>
+      <c r="E39" t="inlineStr">
         <is>
           <t>在群组设置中，存在一个反复清空聊天记录的异常功能。即使当前没有任何聊天记录，用户仍可以点击进行清空操作。这样的设计违背了常规的用户交互逻辑，导致用户的正常使用被干扰，从而影响了用户体验，使得该功能的使用变得不友好。</t>
         </is>
       </c>
-      <c r="B39" t="inlineStr">
+      <c r="F39" t="inlineStr">
         <is>
           <t>群组 设置 反复 清空 聊天记录 异常 当前 没有 聊天记录 点击 进行 清空 设计 违背 常规 交互 逻辑 正常 干扰 变得 友好</t>
         </is>
       </c>
-      <c r="C39" t="inlineStr">
+    </row>
+    <row r="40">
+      <c r="A40" t="n">
+        <v>10010000009157</v>
+      </c>
+      <c r="B40" t="inlineStr">
         <is>
           <t>用户体验</t>
         </is>
       </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
+      <c r="C40" t="n">
+        <v>1</v>
+      </c>
+      <c r="D40" t="n">
+        <v>1</v>
+      </c>
+      <c r="E40" t="inlineStr">
         <is>
           <t>在软件测试中，该问题描述为：当用户尝试加入一个群聊时，之前的聊天记录被后续加入群的用户查看。这违反了用户的隐私权，可能导致敏感信息的泄露。</t>
         </is>
       </c>
-      <c r="B40" t="inlineStr">
+      <c r="F40" t="inlineStr">
         <is>
           <t>软件测试 加入 群聊 之前 聊天记录 后续 加入 群 查看 违反 隐私权 敏感 信息 泄露</t>
         </is>
       </c>
-      <c r="C40" t="inlineStr">
+    </row>
+    <row r="41">
+      <c r="A41" t="n">
+        <v>10010000008976</v>
+      </c>
+      <c r="B41" t="inlineStr">
         <is>
           <t>用户体验</t>
         </is>
       </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
+      <c r="C41" t="n">
+        <v>3</v>
+      </c>
+      <c r="D41" t="n">
+        <v>5</v>
+      </c>
+      <c r="E41" t="inlineStr">
         <is>
           <t>该软件界面中存在一个明显的用户交互问题，即“可以反复删除群组设置的聊天记录”，这导致用户体验极差。用户在尝试删除或查看已设定的群组聊天记录时，系统似乎没有提供正确的反馈或限制，使得用户可以无限制地重复此过程。这不仅消耗了用户的时间和资源，还可能对用户造成不必要的困扰和混淆。</t>
         </is>
       </c>
-      <c r="B41" t="inlineStr">
+      <c r="F41" t="inlineStr">
         <is>
           <t>界面 明显 交互 反复 删除 群组 设置 聊天记录 极差 删除 查看 设定 群组 聊天记录 系统 没有 提供 正确 反馈 限制 限制 重复 过程 消耗 时间 资源 造成 不必要 困扰 混淆</t>
         </is>
       </c>
-      <c r="C41" t="inlineStr">
+    </row>
+    <row r="42">
+      <c r="A42" t="n">
+        <v>10010000009587</v>
+      </c>
+      <c r="B42" t="inlineStr">
         <is>
           <t>用户体验</t>
         </is>
       </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
+      <c r="C42" t="n">
+        <v>4</v>
+      </c>
+      <c r="D42" t="n">
+        <v>5</v>
+      </c>
+      <c r="E42" t="inlineStr">
         <is>
           <t>清空聊天记录，仍然能从聊天记录的历史消息中看到消息记录</t>
         </is>
       </c>
-      <c r="B42" t="inlineStr">
+      <c r="F42" t="inlineStr">
         <is>
           <t>清空 聊天记录 仍然 聊天记录 历史 消息 看到 消息 记录</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>用户体验</t>
         </is>
       </c>
     </row>

</xml_diff>